<commit_message>
Task 3 is correct
</commit_message>
<xml_diff>
--- a/Task 3/Planes_Data/B747_FC5.xlsx
+++ b/Task 3/Planes_Data/B747_FC5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\4th year\Second term\Design of Control Systems for Aeronautical and Space Vehicles _ AER4420\Project\Autopilot-project\Task 3\Planes_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636D5CD8-C84B-4DCD-B113-6A6E2489223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39067859-F0AC-4692-9937-A7021ADA4104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1208,7 +1208,7 @@
   <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,7 +2256,7 @@
         <v>136</v>
       </c>
       <c r="B60" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
start in task 4
</commit_message>
<xml_diff>
--- a/Task 3/Planes_Data/B747_FC5.xlsx
+++ b/Task 3/Planes_Data/B747_FC5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\4th year\Second term\Design of Control Systems for Aeronautical and Space Vehicles _ AER4420\Project\Autopilot-project\Task 3\Planes_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39067859-F0AC-4692-9937-A7021ADA4104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E221060B-49B0-4F4A-9E4F-AF245E5C1CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1208,7 +1208,7 @@
   <dimension ref="A1:N70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,7 +2248,7 @@
         <v>135</v>
       </c>
       <c r="B59" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>